<commit_message>
Training for new datasets
</commit_message>
<xml_diff>
--- a/Evaluation/stat.xlsx
+++ b/Evaluation/stat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E-MaxPCShop\PycharmProjects\LetterCubicGame\Evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539BB6F8-4A10-4B8F-AEC7-CEDC9AB4A2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC263FEA-9E61-41E2-B9C6-DF98387BA981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{BEB96F31-1855-48FF-A368-14514A8512CF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BEB96F31-1855-48FF-A368-14514A8512CF}"/>
   </bookViews>
   <sheets>
     <sheet name="uz" sheetId="1" r:id="rId1"/>
@@ -308,16 +308,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -9852,7 +9852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C977221-D0D9-4562-BF56-491B22606DAC}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -10809,7 +10809,7 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K1" sqref="I1:K1"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11685,27 +11685,27 @@
       <c r="F14">
         <v>55</v>
       </c>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
       <c r="L14" s="20"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
       <c r="P14" s="20"/>
-      <c r="Q14" s="25" t="s">
+      <c r="Q14" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27"/>
       <c r="U14" s="20"/>
-      <c r="V14" s="25" t="s">
+      <c r="V14" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="W14" s="25"/>
-      <c r="X14" s="25"/>
-      <c r="Y14" s="25"/>
+      <c r="W14" s="27"/>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
@@ -11883,16 +11883,16 @@
         <v>19</v>
       </c>
       <c r="H19" s="23"/>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="27"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="26" t="s">
+      <c r="J19" s="28"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="27"/>
-      <c r="N19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="26"/>
       <c r="O19" s="19"/>
       <c r="P19"/>
       <c r="T19" s="19"/>
@@ -12142,18 +12142,18 @@
         <v>50.4</v>
       </c>
       <c r="H26" s="23"/>
-      <c r="I26" s="26" t="s">
+      <c r="I26" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="J26" s="28"/>
-      <c r="K26" s="26" t="s">
+      <c r="J26" s="26"/>
+      <c r="K26" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="L26" s="28"/>
-      <c r="M26" s="26" t="s">
+      <c r="L26" s="26"/>
+      <c r="M26" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="N26" s="28"/>
+      <c r="N26" s="26"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="H27" s="23" t="s">
@@ -12416,15 +12416,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="Q14:T14"/>
+    <mergeCell ref="V14:Y14"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L19:N19"/>
     <mergeCell ref="I26:J26"/>
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="M26:N26"/>
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="M14:O14"/>
-    <mergeCell ref="Q14:T14"/>
-    <mergeCell ref="V14:Y14"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="L19:N19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12435,7 +12435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A199716-0BF3-40B4-9C34-5315D9C6F674}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -13756,7 +13756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F52E5A-7EFC-4699-987F-49E8F6DCC9E1}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C32" sqref="C32:F32"/>
     </sheetView>
   </sheetViews>

</xml_diff>